<commit_message>
updates post TE discussion
</commit_message>
<xml_diff>
--- a/processeddata/shock_metadata.xlsx
+++ b/processeddata/shock_metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>country</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>no data??</t>
+  </si>
+  <si>
+    <t>recall_years</t>
+  </si>
+  <si>
+    <t>spatial_representitiveness</t>
+  </si>
+  <si>
+    <t>admin2</t>
   </si>
 </sst>
 </file>
@@ -114,10 +123,25 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,12 +167,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,38 +469,47 @@
     <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -490,16 +528,22 @@
       <c r="F2">
         <v>2015</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -507,7 +551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -515,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -523,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -531,7 +575,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -539,7 +583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -547,7 +591,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -555,7 +599,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -563,7 +607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -571,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -579,7 +623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -598,11 +642,11 @@
       <c r="F14">
         <v>2009</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -621,11 +665,11 @@
       <c r="F15">
         <v>2011</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -645,30 +689,30 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>10</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>2014</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>11</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>2015</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -676,7 +720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -684,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -692,7 +736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -700,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>

</xml_diff>